<commit_message>
nuevas funcionalidades y actualización
</commit_message>
<xml_diff>
--- a/enlaces_equipos.xlsx
+++ b/enlaces_equipos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://v7hfx-my.sharepoint.com/personal/joseca20_v7hfx_onmicrosoft_com/Documents/web scraping/statsFutbol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{C9A4DFC4-E548-46DD-BD70-6930DD5E65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7928AFC7-3A1C-465B-9C5E-74C5AEE6F34A}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{C9A4DFC4-E548-46DD-BD70-6930DD5E65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF8EAACA-B3FF-4F1C-B4B8-A549D35BCBA5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{474EBA83-D6A0-4565-BEB0-BC6B2AA992C1}"/>
   </bookViews>
@@ -872,9 +872,6 @@
     <t>europe/france/as-monaco-fc</t>
   </si>
   <si>
-    <t>europe/france/montpellier-hsc</t>
-  </si>
-  <si>
     <t>europe/france/fc-nantes</t>
   </si>
   <si>
@@ -884,15 +881,9 @@
     <t>europe/france/paris-saint-germain-fc</t>
   </si>
   <si>
-    <t>europe/france/stade-de-reims</t>
-  </si>
-  <si>
     <t>europe/france/stade-rennais-fc</t>
   </si>
   <si>
-    <t>europe/france/as-saint-etienne</t>
-  </si>
-  <si>
     <t>europe/france/rc-strasbourg-alsace</t>
   </si>
   <si>
@@ -965,9 +956,6 @@
     <t>europe/italy/como-1907</t>
   </si>
   <si>
-    <t>europe/italy/empoli-fc</t>
-  </si>
-  <si>
     <t>europe/italy/acf-fiorentina</t>
   </si>
   <si>
@@ -986,9 +974,6 @@
     <t>europe/italy/us-lecce</t>
   </si>
   <si>
-    <t>europe/italy/ac-monza</t>
-  </si>
-  <si>
     <t>europe/italy/ssc-napoli</t>
   </si>
   <si>
@@ -1001,9 +986,6 @@
     <t>europe/italy/udinese-calcio</t>
   </si>
   <si>
-    <t>europe/italy/venezia-fc</t>
-  </si>
-  <si>
     <t>europe/italy/hellas-verona-fc</t>
   </si>
   <si>
@@ -1755,6 +1737,24 @@
   </si>
   <si>
     <t>europe/germany/hamburger-sv</t>
+  </si>
+  <si>
+    <t>europe/italy/us-cremonese</t>
+  </si>
+  <si>
+    <t>europe/italy/ac-pisa-1909</t>
+  </si>
+  <si>
+    <t>europe/italy/us-sassuolo-calcio</t>
+  </si>
+  <si>
+    <t>europe/france/fc-lorient</t>
+  </si>
+  <si>
+    <t>europe/france/fc-metz</t>
+  </si>
+  <si>
+    <t>europe/france/paris-fc</t>
   </si>
 </sst>
 </file>
@@ -1876,10 +1876,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2197,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC3E121-4DD2-4C5A-A60B-ED62DD98B116}">
   <dimension ref="A1:C592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="B304" sqref="B304:B321"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268:B285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5759,10 +5755,10 @@
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>olympique-lyonnais</v>
+        <v>fc-lorient</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>275</v>
+        <v>570</v>
       </c>
       <c r="C274" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5772,10 +5768,10 @@
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>olympique-de-marseille</v>
+        <v>olympique-lyonnais</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C275" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5785,10 +5781,10 @@
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>as-monaco-fc</v>
+        <v>olympique-de-marseille</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C276" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5798,10 +5794,10 @@
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>montpellier-hsc</v>
+        <v>fc-metz</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>278</v>
+        <v>571</v>
       </c>
       <c r="C277" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5811,10 +5807,10 @@
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>fc-nantes</v>
+        <v>as-monaco-fc</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C278" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5824,10 +5820,10 @@
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>ogc-nice</v>
+        <v>fc-nantes</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C279" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5837,10 +5833,10 @@
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>paris-saint-germain-fc</v>
+        <v>ogc-nice</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C280" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5850,10 +5846,10 @@
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>stade-de-reims</v>
+        <v>paris-fc</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>282</v>
+        <v>572</v>
       </c>
       <c r="C281" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5863,10 +5859,10 @@
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>stade-rennais-fc</v>
+        <v>paris-saint-germain-fc</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C282" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5876,10 +5872,10 @@
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>as-saint-etienne</v>
+        <v>stade-rennais-fc</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C283" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5892,7 +5888,7 @@
         <v>rc-strasbourg-alsace</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C284" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5905,7 +5901,7 @@
         <v>toulouse-fc</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C285" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -5970,7 +5966,7 @@
         <v>fc-koln</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="C290" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6009,7 +6005,7 @@
         <v>hamburger-sv</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="C293" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6152,7 +6148,7 @@
         <v>arminia-bielefeld</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C304" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6178,7 +6174,7 @@
         <v>eintracht-braunschweig</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C306" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6191,7 +6187,7 @@
         <v>darmstadt-98</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C307" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6204,7 +6200,7 @@
         <v>dynamo-dresden</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C308" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6217,7 +6213,7 @@
         <v>fortuna-dusseldorf</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C309" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6230,7 +6226,7 @@
         <v>sv-elversberg</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C310" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6243,7 +6239,7 @@
         <v>greuther-furth</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C311" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6256,7 +6252,7 @@
         <v>hannover-96</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C312" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6269,7 +6265,7 @@
         <v>hertha-berlin</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C313" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6282,7 +6278,7 @@
         <v>fc-kaiserslautern</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C314" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6295,7 +6291,7 @@
         <v>karlsruher-sc</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C315" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6321,7 +6317,7 @@
         <v>fc-magdeburg</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C317" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6334,7 +6330,7 @@
         <v>preussen-munster</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C318" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6347,7 +6343,7 @@
         <v>fc-nurnberg</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C319" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6360,7 +6356,7 @@
         <v>sc-paderborn</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C320" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6373,7 +6369,7 @@
         <v>schalke-04</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C321" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6386,7 +6382,7 @@
         <v>ac-milan</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C322" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6399,7 +6395,7 @@
         <v>as-roma</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C323" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6412,7 +6408,7 @@
         <v>atalanta-bc</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C324" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6425,7 +6421,7 @@
         <v>bologna-fc-1909</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C325" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6438,7 +6434,7 @@
         <v>cagliari-calcio</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C326" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6451,7 +6447,7 @@
         <v>como-1907</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C327" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6461,10 +6457,10 @@
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>empoli-fc</v>
+        <v>us-cremonese</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>309</v>
+        <v>567</v>
       </c>
       <c r="C328" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6477,7 +6473,7 @@
         <v>acf-fiorentina</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C329" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6490,7 +6486,7 @@
         <v>genoa-cfc</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C330" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6503,7 +6499,7 @@
         <v>inter-milan</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C331" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6516,7 +6512,7 @@
         <v>juventus-fc</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C332" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6529,7 +6525,7 @@
         <v>ss-lazio</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C333" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6542,7 +6538,7 @@
         <v>us-lecce</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C334" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6552,10 +6548,10 @@
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>ac-monza</v>
+        <v>ssc-napoli</v>
       </c>
       <c r="B335" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C335" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6565,10 +6561,10 @@
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>ssc-napoli</v>
+        <v>parma-calcio-1913</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C336" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6578,10 +6574,10 @@
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>parma-calcio-1913</v>
+        <v>ac-pisa-1909</v>
       </c>
       <c r="B337" s="5" t="s">
-        <v>318</v>
+        <v>568</v>
       </c>
       <c r="C337" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6591,10 +6587,10 @@
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>torino-fc</v>
+        <v>us-sassuolo-calcio</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>319</v>
+        <v>569</v>
       </c>
       <c r="C338" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6604,10 +6600,10 @@
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>udinese-calcio</v>
+        <v>torino-fc</v>
       </c>
       <c r="B339" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C339" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6617,10 +6613,10 @@
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="str">
         <f>MID(Tabla1[[#This Row],[ENLACE]],FIND("~",SUBSTITUTE(Tabla1[[#This Row],[ENLACE]],"/","~",2))+1,LEN(Tabla1[[#This Row],[ENLACE]]))</f>
-        <v>venezia-fc</v>
+        <v>udinese-calcio</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C340" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6633,7 +6629,7 @@
         <v>hellas-verona-fc</v>
       </c>
       <c r="B341" s="5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C341" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6646,7 +6642,7 @@
         <v>atletico-san-luis</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C342" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6659,7 +6655,7 @@
         <v>atlas-fc</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C343" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6672,7 +6668,7 @@
         <v>club-america</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C344" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6685,7 +6681,7 @@
         <v>cruz-azul</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C345" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6698,7 +6694,7 @@
         <v>cd-guadalajara</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C346" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6711,7 +6707,7 @@
         <v>fc-juarez</v>
       </c>
       <c r="B347" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C347" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6724,7 +6720,7 @@
         <v>club-leon</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C348" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6737,7 +6733,7 @@
         <v>mazatlan-fc</v>
       </c>
       <c r="B349" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C349" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6750,7 +6746,7 @@
         <v>cf-monterrey</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C350" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6763,7 +6759,7 @@
         <v>club-necaxa</v>
       </c>
       <c r="B351" s="5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C351" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6776,7 +6772,7 @@
         <v>cf-pachuca</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C352" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6789,7 +6785,7 @@
         <v>club-puebla</v>
       </c>
       <c r="B353" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C353" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6802,7 +6798,7 @@
         <v>queretaro-fc</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C354" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6815,7 +6811,7 @@
         <v>santos-laguna</v>
       </c>
       <c r="B355" s="5" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C355" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6828,7 +6824,7 @@
         <v>tigres-uanl</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C356" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6841,7 +6837,7 @@
         <v>club-tijuana</v>
       </c>
       <c r="B357" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C357" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6854,7 +6850,7 @@
         <v>deportivo-toluca-fc</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C358" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6867,7 +6863,7 @@
         <v>unam</v>
       </c>
       <c r="B359" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C359" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6880,7 +6876,7 @@
         <v>afc-ajax</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C360" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6893,7 +6889,7 @@
         <v>az-alkmaar</v>
       </c>
       <c r="B361" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C361" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6906,7 +6902,7 @@
         <v>sbv-excelsior</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C362" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6919,7 +6915,7 @@
         <v>fc-volendam</v>
       </c>
       <c r="B363" s="5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C363" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6932,7 +6928,7 @@
         <v>feyenoord-rotterdam</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C364" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6945,7 +6941,7 @@
         <v>go-ahead-eagles</v>
       </c>
       <c r="B365" s="5" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C365" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6958,7 +6954,7 @@
         <v>fc-groningen</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C366" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6971,7 +6967,7 @@
         <v>sc-heerenveen</v>
       </c>
       <c r="B367" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C367" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6984,7 +6980,7 @@
         <v>heracles-almelo</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C368" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -6997,7 +6993,7 @@
         <v>nac-breda</v>
       </c>
       <c r="B369" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C369" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7010,7 +7006,7 @@
         <v>nec-nijmegen</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C370" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7023,7 +7019,7 @@
         <v>psv-eindhoven</v>
       </c>
       <c r="B371" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C371" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7036,7 +7032,7 @@
         <v>fortuna-sittard</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C372" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7049,7 +7045,7 @@
         <v>sparta-rotterdam</v>
       </c>
       <c r="B373" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C373" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7062,7 +7058,7 @@
         <v>sc-telstar</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C374" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7075,7 +7071,7 @@
         <v>fc-twente</v>
       </c>
       <c r="B375" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C375" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7088,7 +7084,7 @@
         <v>fc-utrecht</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C376" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7101,7 +7097,7 @@
         <v>pec-zwolle</v>
       </c>
       <c r="B377" s="5" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C377" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7114,7 +7110,7 @@
         <v>fk-bodo-glimt</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C378" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7127,7 +7123,7 @@
         <v>sk-brann</v>
       </c>
       <c r="B379" s="5" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C379" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7140,7 +7136,7 @@
         <v>bryne-fk</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C380" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7153,7 +7149,7 @@
         <v>fredrikstad-fk</v>
       </c>
       <c r="B381" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C381" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7166,7 +7162,7 @@
         <v>ham-kam</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C382" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7179,7 +7175,7 @@
         <v>fk-haugesund</v>
       </c>
       <c r="B383" s="5" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C383" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7192,7 +7188,7 @@
         <v>kfum-kameratene-oslo</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C384" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7205,7 +7201,7 @@
         <v>kristiansund-bk</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C385" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7218,7 +7214,7 @@
         <v>molde-fk</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C386" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7231,7 +7227,7 @@
         <v>rosenborg-bk</v>
       </c>
       <c r="B387" s="5" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C387" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7244,7 +7240,7 @@
         <v>sandefjord-fotball</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C388" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7257,7 +7253,7 @@
         <v>sarpsborg-08-ff</v>
       </c>
       <c r="B389" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C389" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7270,7 +7266,7 @@
         <v>stromsgodset</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C390" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7283,7 +7279,7 @@
         <v>tromso-il</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C391" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7296,7 +7292,7 @@
         <v>valerenga-fotball</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C392" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7309,7 +7305,7 @@
         <v>viking-fk</v>
       </c>
       <c r="B393" s="5" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C393" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7322,7 +7318,7 @@
         <v>alianza-lima</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C394" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7335,7 +7331,7 @@
         <v>asociacion-deportiva-tarma</v>
       </c>
       <c r="B395" s="5" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C395" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7348,7 +7344,7 @@
         <v>alianza-atletico</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C396" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7361,7 +7357,7 @@
         <v>alianza-universidad-de-huanuco</v>
       </c>
       <c r="B397" s="5" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C397" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7374,7 +7370,7 @@
         <v>ayacucho-fc</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C398" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7387,7 +7383,7 @@
         <v>deportivo-binacional</v>
       </c>
       <c r="B399" s="5" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C399" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7400,7 +7396,7 @@
         <v>universidad-tecnica-de-cajamarca</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C400" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7413,7 +7409,7 @@
         <v>club-sportivo-cienciano</v>
       </c>
       <c r="B401" s="5" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C401" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7426,7 +7422,7 @@
         <v>comerciantes-unidos</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C402" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7439,7 +7435,7 @@
         <v>cusco-fc</v>
       </c>
       <c r="B403" s="5" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C403" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7452,7 +7448,7 @@
         <v>deportivo-garcilaso</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C404" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7465,7 +7461,7 @@
         <v>atletico-grau</v>
       </c>
       <c r="B405" s="5" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C405" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7478,7 +7474,7 @@
         <v>sport-huancayo</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C406" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7491,7 +7487,7 @@
         <v>adc-juan-pablo-ii-college</v>
       </c>
       <c r="B407" s="5" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C407" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7504,7 +7500,7 @@
         <v>los-chankas-cyc</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C408" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7517,7 +7513,7 @@
         <v>fbc-melgar</v>
       </c>
       <c r="B409" s="5" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C409" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7530,7 +7526,7 @@
         <v>sport-boys</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C410" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7543,7 +7539,7 @@
         <v>sporting-cristal</v>
       </c>
       <c r="B411" s="5" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C411" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7556,7 +7552,7 @@
         <v>club-universitario-de-deportes</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C412" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7569,7 +7565,7 @@
         <v>arka-gdynia</v>
       </c>
       <c r="B413" s="5" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C413" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7582,7 +7578,7 @@
         <v>cracovia</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C414" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7595,7 +7591,7 @@
         <v>gornik-zabrze</v>
       </c>
       <c r="B415" s="5" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C415" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7608,7 +7604,7 @@
         <v>jagiellona-bialystok</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C416" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7621,7 +7617,7 @@
         <v>gks-katowice</v>
       </c>
       <c r="B417" s="5" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C417" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7634,7 +7630,7 @@
         <v>korona-kielce</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C418" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7647,7 +7643,7 @@
         <v>lech-poznan</v>
       </c>
       <c r="B419" s="5" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C419" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7660,7 +7656,7 @@
         <v>lechia-gdansk</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C420" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7673,7 +7669,7 @@
         <v>legia-warsaw</v>
       </c>
       <c r="B421" s="5" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C421" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7686,7 +7682,7 @@
         <v>motor-lublin</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C422" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7699,7 +7695,7 @@
         <v>piast-gliwice</v>
       </c>
       <c r="B423" s="5" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C423" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7712,7 +7708,7 @@
         <v>mks-pogon-szczecin</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C424" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7725,7 +7721,7 @@
         <v>radomiak-radom</v>
       </c>
       <c r="B425" s="5" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C425" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7738,7 +7734,7 @@
         <v>rakow-czestochowa</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C426" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7751,7 +7747,7 @@
         <v>bruk-bet-termalica-nieciecza</v>
       </c>
       <c r="B427" s="5" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C427" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7764,7 +7760,7 @@
         <v>rts-widzew-lodz</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C428" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7777,7 +7773,7 @@
         <v>wisla-plock</v>
       </c>
       <c r="B429" s="5" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C429" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7790,7 +7786,7 @@
         <v>zaglebie-lubin</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C430" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7803,7 +7799,7 @@
         <v>avs-futebol-sad</v>
       </c>
       <c r="B431" s="5" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C431" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7816,7 +7812,7 @@
         <v>fc-alverca</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="C432" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7829,7 +7825,7 @@
         <v>fc-arouca</v>
       </c>
       <c r="B433" s="5" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C433" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7842,7 +7838,7 @@
         <v>benfica</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C434" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7855,7 +7851,7 @@
         <v>braga</v>
       </c>
       <c r="B435" s="5" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C435" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7868,7 +7864,7 @@
         <v>casa-pia-ac</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="C436" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7881,7 +7877,7 @@
         <v>gd-estoril-praia</v>
       </c>
       <c r="B437" s="5" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C437" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7894,7 +7890,7 @@
         <v>cf-estrela-da-amadora</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C438" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7907,7 +7903,7 @@
         <v>famalicao</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="C439" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7920,7 +7916,7 @@
         <v>fc-porto</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C440" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7933,7 +7929,7 @@
         <v>gil-vicente</v>
       </c>
       <c r="B441" s="5" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C441" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7946,7 +7942,7 @@
         <v>vitoria-de-guimaraes</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="C442" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7959,7 +7955,7 @@
         <v>moreirense-fc</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C443" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7972,7 +7968,7 @@
         <v>cd-nacional</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C444" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7985,7 +7981,7 @@
         <v>rio-ave-fc</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="C445" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -7998,7 +7994,7 @@
         <v>santa-clara</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="C446" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8011,7 +8007,7 @@
         <v>sporting-cp</v>
       </c>
       <c r="B447" s="5" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C447" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8024,7 +8020,7 @@
         <v>cd-tondela</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="C448" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8037,7 +8033,7 @@
         <v>fc-botosani</v>
       </c>
       <c r="B449" s="5" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="C449" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8050,7 +8046,7 @@
         <v>cfr-cluj</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C450" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8063,7 +8059,7 @@
         <v>fk-miercurea-ciuc</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C451" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8076,7 +8072,7 @@
         <v>fc-dinamo-bucuresti</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="C452" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8089,7 +8085,7 @@
         <v>fc-farul-constanta</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="C453" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8102,7 +8098,7 @@
         <v>fc-arges-pitesti</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C454" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8115,7 +8111,7 @@
         <v>fc-hermannstadt</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C455" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8128,7 +8124,7 @@
         <v>fc-rapid-bucuresti</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C456" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8141,7 +8137,7 @@
         <v>fcsb</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="C457" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8154,7 +8150,7 @@
         <v>fc-metaloglobus-bucuresti</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C458" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8167,7 +8163,7 @@
         <v>asc-otelul-galati</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="C459" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8180,7 +8176,7 @@
         <v>fc-petrolul-ploiesti</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C460" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8193,7 +8189,7 @@
         <v>fc-universitatea-cluj</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C461" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8206,7 +8202,7 @@
         <v>afc-unirea-slobozia</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C462" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8219,7 +8215,7 @@
         <v>cs-universitatea-craiova</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C463" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8232,7 +8228,7 @@
         <v>fc-uta-arad</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C464" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8245,7 +8241,7 @@
         <v>al-okhdood-club</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="C465" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8258,7 +8254,7 @@
         <v>al-fateh-sc</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C466" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8271,7 +8267,7 @@
         <v>al-fayha-fc</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C467" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8284,7 +8280,7 @@
         <v>khaleej-fc</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C468" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8297,7 +8293,7 @@
         <v>al-kholood-club</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="C469" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8310,7 +8306,7 @@
         <v>al-orobah-fc</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C470" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8323,7 +8319,7 @@
         <v>al-qadsiah-fc</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C471" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8336,7 +8332,7 @@
         <v>al-riyadh-sc</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="C472" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8349,7 +8345,7 @@
         <v>al-ahli-saudi-fc</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C473" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8362,7 +8358,7 @@
         <v>al-ettifaq-fc</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C474" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8375,7 +8371,7 @@
         <v>al-hilal-fc</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="C475" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8388,7 +8384,7 @@
         <v>al-ittihad-fc</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C476" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8401,7 +8397,7 @@
         <v>al-nassr-fc</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C477" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8414,7 +8410,7 @@
         <v>al-raed-fc</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="C478" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8427,7 +8423,7 @@
         <v>al-shabab-fc</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C479" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8440,7 +8436,7 @@
         <v>al-taawoun-fc</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C480" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8453,7 +8449,7 @@
         <v>al-wehda</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C481" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8466,7 +8462,7 @@
         <v>damac-fc</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="C482" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8479,7 +8475,7 @@
         <v>aberdeen-fc</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="C483" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8492,7 +8488,7 @@
         <v>celtic-fc</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C484" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8505,7 +8501,7 @@
         <v>dundee-fc</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="C485" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8518,7 +8514,7 @@
         <v>dundee-united-fc</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C486" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8531,7 +8527,7 @@
         <v>falkirk-fc</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="C487" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8544,7 +8540,7 @@
         <v>heart-of-midlothian-fc</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C488" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8557,7 +8553,7 @@
         <v>hibernian-fc</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C489" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8570,7 +8566,7 @@
         <v>kilmarnock-fc</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C490" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8583,7 +8579,7 @@
         <v>livingston-fc</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="C491" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8596,7 +8592,7 @@
         <v>motherwell-fc</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C492" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8609,7 +8605,7 @@
         <v>rangers-fc</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="C493" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8622,7 +8618,7 @@
         <v>st-mirren-fc</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C494" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8635,7 +8631,7 @@
         <v>albacete-balompie</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="C495" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8648,7 +8644,7 @@
         <v>ud-almeria</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C496" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8661,7 +8657,7 @@
         <v>fc-andorra</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C497" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8674,7 +8670,7 @@
         <v>burgos-cf</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C498" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8687,7 +8683,7 @@
         <v>cadiz-cf</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C499" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8700,7 +8696,7 @@
         <v>cd-castellon</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C500" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8713,7 +8709,7 @@
         <v>ad-ceuta-fc</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="C501" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8726,7 +8722,7 @@
         <v>cordoba-cf</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C502" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8739,7 +8735,7 @@
         <v>cultural-y-deportiva-leonesa</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="C503" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8752,7 +8748,7 @@
         <v>sd-eibar</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C504" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8765,7 +8761,7 @@
         <v>sporting-de-gijon</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="C505" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8778,7 +8774,7 @@
         <v>granada-cf</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="C506" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8791,7 +8787,7 @@
         <v>sd-huesca</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="C507" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8804,7 +8800,7 @@
         <v>deportivo-de-la-coruna</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="C508" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8843,7 +8839,7 @@
         <v>malaga-cf</v>
       </c>
       <c r="B511" s="5" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="C511" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8856,7 +8852,7 @@
         <v>cd-mirandes</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="C512" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8869,7 +8865,7 @@
         <v>racing-de-santander</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="C513" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8882,7 +8878,7 @@
         <v>real-sociedad-b</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="C514" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8908,7 +8904,7 @@
         <v>real-zaragoza</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="C516" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8921,7 +8917,7 @@
         <v>aik</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="C517" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8934,7 +8930,7 @@
         <v>if-brommapojkarna</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="C518" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8947,7 +8943,7 @@
         <v>degerfors-if</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="C519" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8960,7 +8956,7 @@
         <v>djurgardens-if</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C520" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8973,7 +8969,7 @@
         <v>if-elfsborg</v>
       </c>
       <c r="B521" s="5" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="C521" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8986,7 +8982,7 @@
         <v>gais</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="C522" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -8999,7 +8995,7 @@
         <v>ifk-goteborg</v>
       </c>
       <c r="B523" s="5" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="C523" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9012,7 +9008,7 @@
         <v>bk-hacken</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="C524" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9025,7 +9021,7 @@
         <v>halmstads-bk</v>
       </c>
       <c r="B525" s="5" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C525" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9038,7 +9034,7 @@
         <v>hammarby-if</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="C526" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9051,7 +9047,7 @@
         <v>malmo-ff</v>
       </c>
       <c r="B527" s="5" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C527" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9064,7 +9060,7 @@
         <v>mjallby-aif</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="C528" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9077,7 +9073,7 @@
         <v>ifk-norrkoping</v>
       </c>
       <c r="B529" s="5" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C529" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9090,7 +9086,7 @@
         <v>osters-if</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="C530" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9103,7 +9099,7 @@
         <v>ik-sirius</v>
       </c>
       <c r="B531" s="5" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C531" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9116,7 +9112,7 @@
         <v>ifk-varnamo</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="C532" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9129,7 +9125,7 @@
         <v>fc-basel</v>
       </c>
       <c r="B533" s="5" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C533" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9142,7 +9138,7 @@
         <v>grasshopper-club-zurich</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="C534" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9155,7 +9151,7 @@
         <v>fc-lausanne-sport</v>
       </c>
       <c r="B535" s="5" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C535" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9168,7 +9164,7 @@
         <v>fc-lugano</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C536" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9181,7 +9177,7 @@
         <v>fc-luzern</v>
       </c>
       <c r="B537" s="5" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C537" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9194,7 +9190,7 @@
         <v>servette-fc</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C538" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9207,7 +9203,7 @@
         <v>fc-sion</v>
       </c>
       <c r="B539" s="5" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="C539" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9220,7 +9216,7 @@
         <v>fc-st-gallen</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C540" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9233,7 +9229,7 @@
         <v>fc-thun</v>
       </c>
       <c r="B541" s="5" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="C541" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9246,7 +9242,7 @@
         <v>fc-winterthur</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C542" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9259,7 +9255,7 @@
         <v>bsc-young-boys</v>
       </c>
       <c r="B543" s="5" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="C543" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9272,7 +9268,7 @@
         <v>fc-zurich</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C544" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9285,7 +9281,7 @@
         <v>alanyaspor</v>
       </c>
       <c r="B545" s="5" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C545" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9298,7 +9294,7 @@
         <v>antalyaspor</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C546" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9311,7 +9307,7 @@
         <v>istanbul-basaksehir-fk</v>
       </c>
       <c r="B547" s="5" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C547" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9324,7 +9320,7 @@
         <v>besiktas-jk</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C548" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9337,7 +9333,7 @@
         <v>eyupspor</v>
       </c>
       <c r="B549" s="5" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C549" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9350,7 +9346,7 @@
         <v>fenerbahce-sk</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="C550" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9363,7 +9359,7 @@
         <v>galatasaray-sk</v>
       </c>
       <c r="B551" s="5" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C551" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9376,7 +9372,7 @@
         <v>gaziantep-fk</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C552" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9389,7 +9385,7 @@
         <v>genclerbirligi-sk</v>
       </c>
       <c r="B553" s="5" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C553" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9402,7 +9398,7 @@
         <v>goztepe-sk</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C554" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9415,7 +9411,7 @@
         <v>fatih-karagumruk-sk</v>
       </c>
       <c r="B555" s="5" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C555" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9428,7 +9424,7 @@
         <v>kasimpasa-sk</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C556" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9441,7 +9437,7 @@
         <v>kayserispor</v>
       </c>
       <c r="B557" s="5" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C557" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9454,7 +9450,7 @@
         <v>kocaelispor</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C558" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9467,7 +9463,7 @@
         <v>konyaspor</v>
       </c>
       <c r="B559" s="5" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="C559" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9480,7 +9476,7 @@
         <v>caykur-rizespor</v>
       </c>
       <c r="B560" s="2" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C560" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9493,7 +9489,7 @@
         <v>samsunspor</v>
       </c>
       <c r="B561" s="5" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C561" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9506,7 +9502,7 @@
         <v>trabzonspor</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C562" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9519,7 +9515,7 @@
         <v>atlanta-united-fc</v>
       </c>
       <c r="B563" s="5" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C563" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9532,7 +9528,7 @@
         <v>austin-fc</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="C564" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9545,7 +9541,7 @@
         <v>club-de-foot-montreal</v>
       </c>
       <c r="B565" s="5" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C565" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9558,7 +9554,7 @@
         <v>charlotte-fc</v>
       </c>
       <c r="B566" s="2" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C566" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9571,7 +9567,7 @@
         <v>chicago-fire-fc</v>
       </c>
       <c r="B567" s="5" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="C567" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9584,7 +9580,7 @@
         <v>fc-cincinnati</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="C568" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9597,7 +9593,7 @@
         <v>colorado-rapids</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C569" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9610,7 +9606,7 @@
         <v>columbus-crew-sc</v>
       </c>
       <c r="B570" s="2" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="C570" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9623,7 +9619,7 @@
         <v>dc-united</v>
       </c>
       <c r="B571" s="5" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="C571" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9636,7 +9632,7 @@
         <v>fc-dallas</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="C572" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9649,7 +9645,7 @@
         <v>houston-dynamo</v>
       </c>
       <c r="B573" s="5" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="C573" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9662,7 +9658,7 @@
         <v>inter-miami-cf</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="C574" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9675,7 +9671,7 @@
         <v>los-angeles-fc</v>
       </c>
       <c r="B575" s="5" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C575" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9688,7 +9684,7 @@
         <v>los-angeles-galaxy</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="C576" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9701,7 +9697,7 @@
         <v>minnesota-united-fc</v>
       </c>
       <c r="B577" s="5" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C577" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9714,7 +9710,7 @@
         <v>nashville-sc</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="C578" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9727,7 +9723,7 @@
         <v>new-england-revolution</v>
       </c>
       <c r="B579" s="5" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="C579" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9740,7 +9736,7 @@
         <v>new-york-city-fc</v>
       </c>
       <c r="B580" s="2" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="C580" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9753,7 +9749,7 @@
         <v>new-york-red-bulls</v>
       </c>
       <c r="B581" s="5" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C581" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9766,7 +9762,7 @@
         <v>orlando-city-sc</v>
       </c>
       <c r="B582" s="2" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C582" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9779,7 +9775,7 @@
         <v>philadelphia-union</v>
       </c>
       <c r="B583" s="5" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="C583" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9792,7 +9788,7 @@
         <v>portland-timbers</v>
       </c>
       <c r="B584" s="2" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="C584" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9805,7 +9801,7 @@
         <v>real-salt-lake</v>
       </c>
       <c r="B585" s="5" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C585" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9818,7 +9814,7 @@
         <v>san-diego-fc</v>
       </c>
       <c r="B586" s="2" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="C586" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9831,7 +9827,7 @@
         <v>san-jose-earthquakes</v>
       </c>
       <c r="B587" s="5" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C587" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9844,7 +9840,7 @@
         <v>seattle-sounders-fc</v>
       </c>
       <c r="B588" s="2" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="C588" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9857,7 +9853,7 @@
         <v>sporting-kansas-city</v>
       </c>
       <c r="B589" s="5" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C589" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9870,7 +9866,7 @@
         <v>st-louis-city-sc</v>
       </c>
       <c r="B590" s="2" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C590" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9883,7 +9879,7 @@
         <v>toronto-fc</v>
       </c>
       <c r="B591" s="5" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C591" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>
@@ -9896,7 +9892,7 @@
         <v>vancouver-whitecaps-fc</v>
       </c>
       <c r="B592" s="6" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="C592" t="str">
         <f>_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(Tabla1[[#This Row],[ENLACE]],"/",1),"/")</f>

</xml_diff>